<commit_message>
Inclusao da documentação finalizada e do arquivo Word com evidencias de casos de teste
</commit_message>
<xml_diff>
--- a/documentacao/Levantamento de Requisítos.xlsx
+++ b/documentacao/Levantamento de Requisítos.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
-  <si>
-    <t xml:space="preserve">CheckList</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t xml:space="preserve">Requisitos Funcionais</t>
   </si>
@@ -103,7 +100,7 @@
     <t xml:space="preserve">RF005</t>
   </si>
   <si>
-    <t xml:space="preserve">Sistema</t>
+    <t xml:space="preserve">Usuários</t>
   </si>
   <si>
     <t xml:space="preserve">Alertas</t>
@@ -297,32 +294,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -575,10 +576,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="B1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,225 +588,224 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="32.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="45.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -813,61 +813,67 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F25" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E21:F21"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>